<commit_message>
Some edits on the formatting of the Gantt chart
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\ENGR489\QuickCheck for Whiley\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{5D857B35-D930-43A0-A0C1-2E9E47F39350}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F1D348-C8DB-4591-BEBA-050FF38CC0BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
-    <sheet name="About" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$25</definedName>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -81,9 +80,6 @@
   <si>
     <t>ASSIGNED
 TO</t>
-  </si>
-  <si>
-    <t>Project Management Templates</t>
   </si>
   <si>
     <t>START</t>
@@ -99,42 +95,6 @@
   </si>
   <si>
     <t>TASK</t>
-  </si>
-  <si>
-    <t>More Project Management Templates</t>
-  </si>
-  <si>
-    <t>About This Template</t>
-  </si>
-  <si>
-    <t>SIMPLE GANTT CHART by Vertex42.com</t>
-  </si>
-  <si>
-    <t>Additional Help</t>
-  </si>
-  <si>
-    <t>About Vertex42</t>
-  </si>
-  <si>
-    <t>Vertex42.com provides over 300 professionally designed spreadsheet templates for business, home, and education - most of which are free to download. Their collection includes a variety of calendars, planners, and schedules as well as personal finance spreadsheets for budgeting, debt reduction, and loan amortization.</t>
-  </si>
-  <si>
-    <t>Businesses will find invoices, time sheets, inventory trackers, financial statements, and project planning templates. Teachers and students will find resources such as class schedules, grade books, and attendance sheets. Organize your family life with meal planners, checklists, and exercise logs. Each template is thoroughly researched, refined, and improved over time through feedback from thousands of users.</t>
-  </si>
-  <si>
-    <t>https://www.vertex42.com/ExcelTemplates/simple-gantt-chart.html</t>
-  </si>
-  <si>
-    <t>Visit Vertex42.com to download other project management templates, including different types of project schedules, Gantt charts, tasks lists, etc.</t>
-  </si>
-  <si>
-    <t>How to Use the Simple Gantt Chart</t>
-  </si>
-  <si>
-    <t>This template provides a simple way to create a Gantt chart to help visualize and track your project. Simply enter your tasks and start and end dates - no formulas required. The bars in the Gantt chart represent the duration of the task and are displayed using conditional formatting. Insert new tasks by inserting new rows.</t>
-  </si>
-  <si>
-    <t>Click on the link below to visit vertex42.com and learn more about how to use this template, such as how to calculate days and work days, create task dependencies, change the colors of the bars, add a scroll bar to make it easier to change the display week, extend the date range displayed in the chart, etc.</t>
   </si>
   <si>
     <t>Janice Chin</t>
@@ -197,9 +157,9 @@
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
-    <numFmt numFmtId="170" formatCode="d/mm/yy;@"/>
+    <numFmt numFmtId="168" formatCode="d/mm/yy;@"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,49 +300,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
@@ -594,7 +511,7 @@
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -741,40 +658,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="168" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="168" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -789,18 +686,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1065,62 +950,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1905000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>523875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="190500" y="95250"/>
-          <a:ext cx="1905000" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1393,7 +1222,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E4" sqref="E4"/>
+      <selection pane="topRight" activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1425,59 +1254,84 @@
     <col min="43" max="51" width="3" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="2" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="57" width="2" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="70" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="3" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="81" width="3" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="83" max="85" width="2" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="2" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="89" max="91" width="2" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="94" max="101" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="3" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="104" max="112" width="3" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="2" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="2" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="117" max="120" width="2" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="124" max="131" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="3" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="134" max="142" width="3" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="145" max="148" width="2" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="2" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="2" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="155" max="162" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="3" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="165" max="173" width="3" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="175" max="176" width="2" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="2" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="180" max="183" width="2" bestFit="1" customWidth="1"/>
+    <col min="54" max="56" width="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="58" max="60" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="65" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="68" max="70" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="74" max="75" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="80" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="84" max="86" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="2.5546875" bestFit="1" customWidth="1"/>
+    <col min="89" max="91" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="94" max="96" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="99" max="101" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="105" max="106" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="109" max="111" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="115" max="117" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="120" max="121" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="2.5546875" bestFit="1" customWidth="1"/>
+    <col min="124" max="127" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="130" max="132" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="136" max="137" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="140" max="142" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="146" max="148" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="149" max="152" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="155" max="157" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="160" max="162" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="166" max="167" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="170" max="171" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="172" max="173" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="174" max="179" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="180" max="182" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="2" bestFit="1" customWidth="1"/>
     <col min="184" max="184" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="185" max="185" width="2.33203125" bestFit="1" customWidth="1"/>
     <col min="186" max="193" width="2.6640625" bestFit="1" customWidth="1"/>
@@ -1509,7 +1363,7 @@
   <sheetData>
     <row r="1" spans="1:253" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="16" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1520,378 +1374,378 @@
     </row>
     <row r="2" spans="1:253" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:253" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="60">
         <v>43178</v>
       </c>
-      <c r="F3" s="69"/>
+      <c r="F3" s="61"/>
     </row>
     <row r="4" spans="1:253" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="65">
+      <c r="I4" s="57">
         <f>I5</f>
         <v>43178</v>
       </c>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="65">
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="57">
         <f>P5</f>
         <v>43185</v>
       </c>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="65">
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="57">
         <f>W5</f>
         <v>43192</v>
       </c>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="66"/>
-      <c r="AA4" s="66"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="65">
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="57">
         <f>AD5</f>
         <v>43199</v>
       </c>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="66"/>
-      <c r="AG4" s="66"/>
-      <c r="AH4" s="66"/>
-      <c r="AI4" s="66"/>
-      <c r="AJ4" s="67"/>
-      <c r="AK4" s="65">
+      <c r="AE4" s="58"/>
+      <c r="AF4" s="58"/>
+      <c r="AG4" s="58"/>
+      <c r="AH4" s="58"/>
+      <c r="AI4" s="58"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="57">
         <f>AK5</f>
         <v>43206</v>
       </c>
-      <c r="AL4" s="66"/>
-      <c r="AM4" s="66"/>
-      <c r="AN4" s="66"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="66"/>
-      <c r="AQ4" s="67"/>
-      <c r="AR4" s="65">
+      <c r="AL4" s="58"/>
+      <c r="AM4" s="58"/>
+      <c r="AN4" s="58"/>
+      <c r="AO4" s="58"/>
+      <c r="AP4" s="58"/>
+      <c r="AQ4" s="59"/>
+      <c r="AR4" s="57">
         <f>AR5</f>
         <v>43213</v>
       </c>
-      <c r="AS4" s="66"/>
-      <c r="AT4" s="66"/>
-      <c r="AU4" s="66"/>
-      <c r="AV4" s="66"/>
-      <c r="AW4" s="66"/>
-      <c r="AX4" s="67"/>
-      <c r="AY4" s="65">
+      <c r="AS4" s="58"/>
+      <c r="AT4" s="58"/>
+      <c r="AU4" s="58"/>
+      <c r="AV4" s="58"/>
+      <c r="AW4" s="58"/>
+      <c r="AX4" s="59"/>
+      <c r="AY4" s="57">
         <f>AY5</f>
         <v>43220</v>
       </c>
-      <c r="AZ4" s="66"/>
-      <c r="BA4" s="66"/>
-      <c r="BB4" s="66"/>
-      <c r="BC4" s="66"/>
-      <c r="BD4" s="66"/>
-      <c r="BE4" s="67"/>
-      <c r="BF4" s="65">
+      <c r="AZ4" s="58"/>
+      <c r="BA4" s="58"/>
+      <c r="BB4" s="58"/>
+      <c r="BC4" s="58"/>
+      <c r="BD4" s="58"/>
+      <c r="BE4" s="59"/>
+      <c r="BF4" s="57">
         <f>BF5</f>
         <v>43227</v>
       </c>
-      <c r="BG4" s="66"/>
-      <c r="BH4" s="66"/>
-      <c r="BI4" s="66"/>
-      <c r="BJ4" s="66"/>
-      <c r="BK4" s="66"/>
-      <c r="BL4" s="67"/>
-      <c r="BM4" s="65">
+      <c r="BG4" s="58"/>
+      <c r="BH4" s="58"/>
+      <c r="BI4" s="58"/>
+      <c r="BJ4" s="58"/>
+      <c r="BK4" s="58"/>
+      <c r="BL4" s="59"/>
+      <c r="BM4" s="57">
         <f>BM5</f>
         <v>43234</v>
       </c>
-      <c r="BN4" s="66"/>
-      <c r="BO4" s="66"/>
-      <c r="BP4" s="66"/>
-      <c r="BQ4" s="66"/>
-      <c r="BR4" s="66"/>
-      <c r="BS4" s="67"/>
-      <c r="BT4" s="65">
+      <c r="BN4" s="58"/>
+      <c r="BO4" s="58"/>
+      <c r="BP4" s="58"/>
+      <c r="BQ4" s="58"/>
+      <c r="BR4" s="58"/>
+      <c r="BS4" s="59"/>
+      <c r="BT4" s="57">
         <f>BT5</f>
         <v>43241</v>
       </c>
-      <c r="BU4" s="66"/>
-      <c r="BV4" s="66"/>
-      <c r="BW4" s="66"/>
-      <c r="BX4" s="66"/>
-      <c r="BY4" s="66"/>
-      <c r="BZ4" s="67"/>
-      <c r="CA4" s="65">
+      <c r="BU4" s="58"/>
+      <c r="BV4" s="58"/>
+      <c r="BW4" s="58"/>
+      <c r="BX4" s="58"/>
+      <c r="BY4" s="58"/>
+      <c r="BZ4" s="59"/>
+      <c r="CA4" s="57">
         <f>CA5</f>
         <v>43248</v>
       </c>
-      <c r="CB4" s="66"/>
-      <c r="CC4" s="66"/>
-      <c r="CD4" s="66"/>
-      <c r="CE4" s="66"/>
-      <c r="CF4" s="66"/>
-      <c r="CG4" s="67"/>
-      <c r="CH4" s="65">
+      <c r="CB4" s="58"/>
+      <c r="CC4" s="58"/>
+      <c r="CD4" s="58"/>
+      <c r="CE4" s="58"/>
+      <c r="CF4" s="58"/>
+      <c r="CG4" s="59"/>
+      <c r="CH4" s="57">
         <f>CH5</f>
         <v>43255</v>
       </c>
-      <c r="CI4" s="66"/>
-      <c r="CJ4" s="66"/>
-      <c r="CK4" s="66"/>
-      <c r="CL4" s="66"/>
-      <c r="CM4" s="66"/>
-      <c r="CN4" s="67"/>
-      <c r="CO4" s="65">
+      <c r="CI4" s="58"/>
+      <c r="CJ4" s="58"/>
+      <c r="CK4" s="58"/>
+      <c r="CL4" s="58"/>
+      <c r="CM4" s="58"/>
+      <c r="CN4" s="59"/>
+      <c r="CO4" s="57">
         <f>CO5</f>
         <v>43262</v>
       </c>
-      <c r="CP4" s="66"/>
-      <c r="CQ4" s="66"/>
-      <c r="CR4" s="66"/>
-      <c r="CS4" s="66"/>
-      <c r="CT4" s="66"/>
-      <c r="CU4" s="67"/>
-      <c r="CV4" s="65">
+      <c r="CP4" s="58"/>
+      <c r="CQ4" s="58"/>
+      <c r="CR4" s="58"/>
+      <c r="CS4" s="58"/>
+      <c r="CT4" s="58"/>
+      <c r="CU4" s="59"/>
+      <c r="CV4" s="57">
         <f>CV5</f>
         <v>43269</v>
       </c>
-      <c r="CW4" s="66"/>
-      <c r="CX4" s="66"/>
-      <c r="CY4" s="66"/>
-      <c r="CZ4" s="66"/>
-      <c r="DA4" s="66"/>
-      <c r="DB4" s="67"/>
-      <c r="DC4" s="65">
+      <c r="CW4" s="58"/>
+      <c r="CX4" s="58"/>
+      <c r="CY4" s="58"/>
+      <c r="CZ4" s="58"/>
+      <c r="DA4" s="58"/>
+      <c r="DB4" s="59"/>
+      <c r="DC4" s="57">
         <f>DC5</f>
         <v>43276</v>
       </c>
-      <c r="DD4" s="66"/>
-      <c r="DE4" s="66"/>
-      <c r="DF4" s="66"/>
-      <c r="DG4" s="66"/>
-      <c r="DH4" s="66"/>
-      <c r="DI4" s="67"/>
-      <c r="DJ4" s="65">
+      <c r="DD4" s="58"/>
+      <c r="DE4" s="58"/>
+      <c r="DF4" s="58"/>
+      <c r="DG4" s="58"/>
+      <c r="DH4" s="58"/>
+      <c r="DI4" s="59"/>
+      <c r="DJ4" s="57">
         <f>DJ5</f>
         <v>43283</v>
       </c>
-      <c r="DK4" s="66"/>
-      <c r="DL4" s="66"/>
-      <c r="DM4" s="66"/>
-      <c r="DN4" s="66"/>
-      <c r="DO4" s="66"/>
-      <c r="DP4" s="67"/>
-      <c r="DQ4" s="65">
+      <c r="DK4" s="58"/>
+      <c r="DL4" s="58"/>
+      <c r="DM4" s="58"/>
+      <c r="DN4" s="58"/>
+      <c r="DO4" s="58"/>
+      <c r="DP4" s="59"/>
+      <c r="DQ4" s="57">
         <f>DQ5</f>
         <v>43290</v>
       </c>
-      <c r="DR4" s="66"/>
-      <c r="DS4" s="66"/>
-      <c r="DT4" s="66"/>
-      <c r="DU4" s="66"/>
-      <c r="DV4" s="66"/>
-      <c r="DW4" s="67"/>
-      <c r="DX4" s="65">
+      <c r="DR4" s="58"/>
+      <c r="DS4" s="58"/>
+      <c r="DT4" s="58"/>
+      <c r="DU4" s="58"/>
+      <c r="DV4" s="58"/>
+      <c r="DW4" s="59"/>
+      <c r="DX4" s="57">
         <f>DX5</f>
         <v>43297</v>
       </c>
-      <c r="DY4" s="66"/>
-      <c r="DZ4" s="66"/>
-      <c r="EA4" s="66"/>
-      <c r="EB4" s="66"/>
-      <c r="EC4" s="66"/>
-      <c r="ED4" s="67"/>
-      <c r="EE4" s="65">
+      <c r="DY4" s="58"/>
+      <c r="DZ4" s="58"/>
+      <c r="EA4" s="58"/>
+      <c r="EB4" s="58"/>
+      <c r="EC4" s="58"/>
+      <c r="ED4" s="59"/>
+      <c r="EE4" s="57">
         <f>EE5</f>
         <v>43304</v>
       </c>
-      <c r="EF4" s="66"/>
-      <c r="EG4" s="66"/>
-      <c r="EH4" s="66"/>
-      <c r="EI4" s="66"/>
-      <c r="EJ4" s="66"/>
-      <c r="EK4" s="67"/>
-      <c r="EL4" s="65">
+      <c r="EF4" s="58"/>
+      <c r="EG4" s="58"/>
+      <c r="EH4" s="58"/>
+      <c r="EI4" s="58"/>
+      <c r="EJ4" s="58"/>
+      <c r="EK4" s="59"/>
+      <c r="EL4" s="57">
         <f>EL5</f>
         <v>43311</v>
       </c>
-      <c r="EM4" s="66"/>
-      <c r="EN4" s="66"/>
-      <c r="EO4" s="66"/>
-      <c r="EP4" s="66"/>
-      <c r="EQ4" s="66"/>
-      <c r="ER4" s="67"/>
-      <c r="ES4" s="65">
+      <c r="EM4" s="58"/>
+      <c r="EN4" s="58"/>
+      <c r="EO4" s="58"/>
+      <c r="EP4" s="58"/>
+      <c r="EQ4" s="58"/>
+      <c r="ER4" s="59"/>
+      <c r="ES4" s="57">
         <f>ES5</f>
         <v>43318</v>
       </c>
-      <c r="ET4" s="66"/>
-      <c r="EU4" s="66"/>
-      <c r="EV4" s="66"/>
-      <c r="EW4" s="66"/>
-      <c r="EX4" s="66"/>
-      <c r="EY4" s="67"/>
-      <c r="EZ4" s="65">
+      <c r="ET4" s="58"/>
+      <c r="EU4" s="58"/>
+      <c r="EV4" s="58"/>
+      <c r="EW4" s="58"/>
+      <c r="EX4" s="58"/>
+      <c r="EY4" s="59"/>
+      <c r="EZ4" s="57">
         <f>EZ5</f>
         <v>43325</v>
       </c>
-      <c r="FA4" s="66"/>
-      <c r="FB4" s="66"/>
-      <c r="FC4" s="66"/>
-      <c r="FD4" s="66"/>
-      <c r="FE4" s="66"/>
-      <c r="FF4" s="67"/>
-      <c r="FG4" s="65">
+      <c r="FA4" s="58"/>
+      <c r="FB4" s="58"/>
+      <c r="FC4" s="58"/>
+      <c r="FD4" s="58"/>
+      <c r="FE4" s="58"/>
+      <c r="FF4" s="59"/>
+      <c r="FG4" s="57">
         <f>FG5</f>
         <v>43332</v>
       </c>
-      <c r="FH4" s="66"/>
-      <c r="FI4" s="66"/>
-      <c r="FJ4" s="66"/>
-      <c r="FK4" s="66"/>
-      <c r="FL4" s="66"/>
-      <c r="FM4" s="67"/>
-      <c r="FN4" s="65">
+      <c r="FH4" s="58"/>
+      <c r="FI4" s="58"/>
+      <c r="FJ4" s="58"/>
+      <c r="FK4" s="58"/>
+      <c r="FL4" s="58"/>
+      <c r="FM4" s="59"/>
+      <c r="FN4" s="57">
         <f>FN5</f>
         <v>43339</v>
       </c>
-      <c r="FO4" s="66"/>
-      <c r="FP4" s="66"/>
-      <c r="FQ4" s="66"/>
-      <c r="FR4" s="66"/>
-      <c r="FS4" s="66"/>
-      <c r="FT4" s="67"/>
-      <c r="FU4" s="65">
+      <c r="FO4" s="58"/>
+      <c r="FP4" s="58"/>
+      <c r="FQ4" s="58"/>
+      <c r="FR4" s="58"/>
+      <c r="FS4" s="58"/>
+      <c r="FT4" s="59"/>
+      <c r="FU4" s="57">
         <f>FU5</f>
         <v>43346</v>
       </c>
-      <c r="FV4" s="66"/>
-      <c r="FW4" s="66"/>
-      <c r="FX4" s="66"/>
-      <c r="FY4" s="66"/>
-      <c r="FZ4" s="66"/>
-      <c r="GA4" s="67"/>
-      <c r="GB4" s="65">
+      <c r="FV4" s="58"/>
+      <c r="FW4" s="58"/>
+      <c r="FX4" s="58"/>
+      <c r="FY4" s="58"/>
+      <c r="FZ4" s="58"/>
+      <c r="GA4" s="59"/>
+      <c r="GB4" s="57">
         <f>GB5</f>
         <v>43353</v>
       </c>
-      <c r="GC4" s="66"/>
-      <c r="GD4" s="66"/>
-      <c r="GE4" s="66"/>
-      <c r="GF4" s="66"/>
-      <c r="GG4" s="66"/>
-      <c r="GH4" s="67"/>
-      <c r="GI4" s="65">
+      <c r="GC4" s="58"/>
+      <c r="GD4" s="58"/>
+      <c r="GE4" s="58"/>
+      <c r="GF4" s="58"/>
+      <c r="GG4" s="58"/>
+      <c r="GH4" s="59"/>
+      <c r="GI4" s="57">
         <f>GI5</f>
         <v>43360</v>
       </c>
-      <c r="GJ4" s="66"/>
-      <c r="GK4" s="66"/>
-      <c r="GL4" s="66"/>
-      <c r="GM4" s="66"/>
-      <c r="GN4" s="66"/>
-      <c r="GO4" s="67"/>
-      <c r="GP4" s="65">
+      <c r="GJ4" s="58"/>
+      <c r="GK4" s="58"/>
+      <c r="GL4" s="58"/>
+      <c r="GM4" s="58"/>
+      <c r="GN4" s="58"/>
+      <c r="GO4" s="59"/>
+      <c r="GP4" s="57">
         <f>GP5</f>
         <v>43367</v>
       </c>
-      <c r="GQ4" s="66"/>
-      <c r="GR4" s="66"/>
-      <c r="GS4" s="66"/>
-      <c r="GT4" s="66"/>
-      <c r="GU4" s="66"/>
-      <c r="GV4" s="67"/>
-      <c r="GW4" s="65">
+      <c r="GQ4" s="58"/>
+      <c r="GR4" s="58"/>
+      <c r="GS4" s="58"/>
+      <c r="GT4" s="58"/>
+      <c r="GU4" s="58"/>
+      <c r="GV4" s="59"/>
+      <c r="GW4" s="57">
         <f>GW5</f>
         <v>43374</v>
       </c>
-      <c r="GX4" s="66"/>
-      <c r="GY4" s="66"/>
-      <c r="GZ4" s="66"/>
-      <c r="HA4" s="66"/>
-      <c r="HB4" s="66"/>
-      <c r="HC4" s="67"/>
-      <c r="HD4" s="65">
+      <c r="GX4" s="58"/>
+      <c r="GY4" s="58"/>
+      <c r="GZ4" s="58"/>
+      <c r="HA4" s="58"/>
+      <c r="HB4" s="58"/>
+      <c r="HC4" s="59"/>
+      <c r="HD4" s="57">
         <f>HD5</f>
         <v>43381</v>
       </c>
-      <c r="HE4" s="66"/>
-      <c r="HF4" s="66"/>
-      <c r="HG4" s="66"/>
-      <c r="HH4" s="66"/>
-      <c r="HI4" s="66"/>
-      <c r="HJ4" s="67"/>
-      <c r="HK4" s="65">
+      <c r="HE4" s="58"/>
+      <c r="HF4" s="58"/>
+      <c r="HG4" s="58"/>
+      <c r="HH4" s="58"/>
+      <c r="HI4" s="58"/>
+      <c r="HJ4" s="59"/>
+      <c r="HK4" s="57">
         <f>HK5</f>
         <v>43388</v>
       </c>
-      <c r="HL4" s="66"/>
-      <c r="HM4" s="66"/>
-      <c r="HN4" s="66"/>
-      <c r="HO4" s="66"/>
-      <c r="HP4" s="66"/>
-      <c r="HQ4" s="67"/>
-      <c r="HR4" s="65">
+      <c r="HL4" s="58"/>
+      <c r="HM4" s="58"/>
+      <c r="HN4" s="58"/>
+      <c r="HO4" s="58"/>
+      <c r="HP4" s="58"/>
+      <c r="HQ4" s="59"/>
+      <c r="HR4" s="57">
         <f>HR5</f>
         <v>43395</v>
       </c>
-      <c r="HS4" s="66"/>
-      <c r="HT4" s="66"/>
-      <c r="HU4" s="66"/>
-      <c r="HV4" s="66"/>
-      <c r="HW4" s="66"/>
-      <c r="HX4" s="67"/>
-      <c r="HY4" s="65">
+      <c r="HS4" s="58"/>
+      <c r="HT4" s="58"/>
+      <c r="HU4" s="58"/>
+      <c r="HV4" s="58"/>
+      <c r="HW4" s="58"/>
+      <c r="HX4" s="59"/>
+      <c r="HY4" s="57">
         <f>HY5</f>
         <v>43402</v>
       </c>
-      <c r="HZ4" s="66"/>
-      <c r="IA4" s="66"/>
-      <c r="IB4" s="66"/>
-      <c r="IC4" s="66"/>
-      <c r="ID4" s="66"/>
-      <c r="IE4" s="67"/>
-      <c r="IF4" s="65">
+      <c r="HZ4" s="58"/>
+      <c r="IA4" s="58"/>
+      <c r="IB4" s="58"/>
+      <c r="IC4" s="58"/>
+      <c r="ID4" s="58"/>
+      <c r="IE4" s="59"/>
+      <c r="IF4" s="57">
         <f>IF5</f>
         <v>43409</v>
       </c>
-      <c r="IG4" s="66"/>
-      <c r="IH4" s="66"/>
-      <c r="II4" s="66"/>
-      <c r="IJ4" s="66"/>
-      <c r="IK4" s="66"/>
-      <c r="IL4" s="67"/>
-      <c r="IM4" s="65">
+      <c r="IG4" s="58"/>
+      <c r="IH4" s="58"/>
+      <c r="II4" s="58"/>
+      <c r="IJ4" s="58"/>
+      <c r="IK4" s="58"/>
+      <c r="IL4" s="59"/>
+      <c r="IM4" s="57">
         <f>IM5</f>
         <v>43416</v>
       </c>
-      <c r="IN4" s="66"/>
-      <c r="IO4" s="66"/>
-      <c r="IP4" s="66"/>
-      <c r="IQ4" s="66"/>
-      <c r="IR4" s="66"/>
-      <c r="IS4" s="67"/>
+      <c r="IN4" s="58"/>
+      <c r="IO4" s="58"/>
+      <c r="IP4" s="58"/>
+      <c r="IQ4" s="58"/>
+      <c r="IR4" s="58"/>
+      <c r="IS4" s="59"/>
     </row>
     <row r="5" spans="1:253" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
@@ -2880,7 +2734,7 @@
     <row r="6" spans="1:253" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19"/>
       <c r="B6" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>3</v>
@@ -2889,14 +2743,14 @@
         <v>2</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>6</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I6" s="15" t="str">
         <f t="shared" ref="I6" si="138">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -3043,7 +2897,7 @@
         <v>M</v>
       </c>
       <c r="AS6" s="15" t="str">
-        <f t="shared" ref="AS6:CV6" si="140">LEFT(TEXT(AS5,"ddd"),1)</f>
+        <f t="shared" ref="AS6:BL6" si="140">LEFT(TEXT(AS5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="AT6" s="15" t="str">
@@ -4140,7 +3994,7 @@
     <row r="8" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19"/>
       <c r="B8" s="26" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="28"/>
@@ -4400,16 +4254,16 @@
     <row r="9" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
       <c r="B9" s="31" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33">
         <v>0</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="53">
         <v>43178</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="53">
         <v>43199</v>
       </c>
       <c r="G9" s="25"/>
@@ -4666,16 +4520,16 @@
     <row r="10" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
       <c r="B10" s="31" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33">
         <v>0</v>
       </c>
-      <c r="E10" s="70">
+      <c r="E10" s="53">
         <v>43178</v>
       </c>
-      <c r="F10" s="70">
+      <c r="F10" s="53">
         <v>43199</v>
       </c>
       <c r="G10" s="25"/>
@@ -4932,16 +4786,16 @@
     <row r="11" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
       <c r="B11" s="31" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="33">
         <v>0</v>
       </c>
-      <c r="E11" s="70">
+      <c r="E11" s="53">
         <v>43178</v>
       </c>
-      <c r="F11" s="71">
+      <c r="F11" s="54">
         <v>43206</v>
       </c>
       <c r="G11" s="25"/>
@@ -5198,16 +5052,16 @@
     <row r="12" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="31" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="33">
         <v>0</v>
       </c>
-      <c r="E12" s="71">
+      <c r="E12" s="54">
         <v>43206</v>
       </c>
-      <c r="F12" s="71">
+      <c r="F12" s="54">
         <v>43234</v>
       </c>
       <c r="G12" s="25"/>
@@ -5464,16 +5318,16 @@
     <row r="13" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
       <c r="B13" s="31" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="33">
         <v>0</v>
       </c>
-      <c r="E13" s="70">
+      <c r="E13" s="53">
         <v>43234</v>
       </c>
-      <c r="F13" s="71">
+      <c r="F13" s="54">
         <v>43261</v>
       </c>
       <c r="G13" s="25"/>
@@ -5727,16 +5581,16 @@
     <row r="14" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="31" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33">
         <v>0</v>
       </c>
-      <c r="E14" s="71">
+      <c r="E14" s="54">
         <v>43262</v>
       </c>
-      <c r="F14" s="71">
+      <c r="F14" s="54">
         <v>43283</v>
       </c>
       <c r="G14" s="25"/>
@@ -5993,7 +5847,7 @@
     <row r="15" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="34" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C15" s="35"/>
       <c r="D15" s="36"/>
@@ -6253,16 +6107,16 @@
     <row r="16" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="39" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="41">
         <v>0</v>
       </c>
-      <c r="E16" s="72">
+      <c r="E16" s="55">
         <v>43283</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="56">
         <v>43297</v>
       </c>
       <c r="G16" s="25"/>
@@ -6519,16 +6373,16 @@
     <row r="17" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="39" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="41">
         <v>0</v>
       </c>
-      <c r="E17" s="72">
+      <c r="E17" s="55">
         <v>43297</v>
       </c>
-      <c r="F17" s="73">
+      <c r="F17" s="56">
         <v>43318</v>
       </c>
       <c r="G17" s="25"/>
@@ -6785,16 +6639,16 @@
     <row r="18" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
       <c r="B18" s="39" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="41">
         <v>0</v>
       </c>
-      <c r="E18" s="73">
+      <c r="E18" s="56">
         <v>43318</v>
       </c>
-      <c r="F18" s="73">
+      <c r="F18" s="56">
         <v>43358</v>
       </c>
       <c r="G18" s="25"/>
@@ -7051,16 +6905,16 @@
     <row r="19" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="39" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="41">
         <v>0</v>
       </c>
-      <c r="E19" s="73">
+      <c r="E19" s="56">
         <v>43358</v>
       </c>
-      <c r="F19" s="73">
+      <c r="F19" s="56">
         <v>43378</v>
       </c>
       <c r="G19" s="25"/>
@@ -7317,16 +7171,16 @@
     <row r="20" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
       <c r="B20" s="39" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="41">
         <v>0</v>
       </c>
-      <c r="E20" s="72">
+      <c r="E20" s="55">
         <v>43379</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="56">
         <v>43394</v>
       </c>
       <c r="G20" s="25"/>
@@ -7580,16 +7434,16 @@
     <row r="21" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
       <c r="B21" s="39" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="41">
         <v>0</v>
       </c>
-      <c r="E21" s="73">
+      <c r="E21" s="56">
         <v>43395</v>
       </c>
-      <c r="F21" s="73">
+      <c r="F21" s="56">
         <v>43420</v>
       </c>
       <c r="G21" s="25"/>
@@ -8884,7 +8738,7 @@
     <row r="27" spans="1:253" x14ac:dyDescent="0.3">
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
-      <c r="F27" s="64">
+      <c r="F27" s="52">
         <v>43113</v>
       </c>
     </row>
@@ -8894,33 +8748,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="IF4:IL4"/>
-    <mergeCell ref="IM4:IS4"/>
-    <mergeCell ref="GW4:HC4"/>
-    <mergeCell ref="HD4:HJ4"/>
-    <mergeCell ref="HK4:HQ4"/>
-    <mergeCell ref="HR4:HX4"/>
-    <mergeCell ref="HY4:IE4"/>
-    <mergeCell ref="FN4:FT4"/>
-    <mergeCell ref="FU4:GA4"/>
-    <mergeCell ref="GB4:GH4"/>
-    <mergeCell ref="GI4:GO4"/>
-    <mergeCell ref="GP4:GV4"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="EZ4:FF4"/>
-    <mergeCell ref="FG4:FM4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
@@ -8930,6 +8757,33 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="EZ4:FF4"/>
+    <mergeCell ref="FG4:FM4"/>
+    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="FU4:GA4"/>
+    <mergeCell ref="GB4:GH4"/>
+    <mergeCell ref="GI4:GO4"/>
+    <mergeCell ref="GP4:GV4"/>
+    <mergeCell ref="IF4:IL4"/>
+    <mergeCell ref="IM4:IS4"/>
+    <mergeCell ref="GW4:HC4"/>
+    <mergeCell ref="HD4:HJ4"/>
+    <mergeCell ref="HK4:HQ4"/>
+    <mergeCell ref="HR4:HX4"/>
+    <mergeCell ref="HY4:IE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D25">
     <cfRule type="dataBar" priority="54">
@@ -9002,115 +8856,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:C19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.88671875" style="53" customWidth="1"/>
-    <col min="2" max="2" width="87.109375" style="60" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="53"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="52"/>
-    </row>
-    <row r="2" spans="2:3" s="55" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="54"/>
-    </row>
-    <row r="3" spans="2:3" s="57" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="56"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="52"/>
-    </row>
-    <row r="5" spans="2:3" s="58" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B5" s="61" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="62" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B7" s="59"/>
-    </row>
-    <row r="8" spans="2:3" s="58" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B8" s="61" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="62" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="63" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="59"/>
-    </row>
-    <row r="12" spans="2:3" s="58" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B12" s="61" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B14" s="63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="59"/>
-    </row>
-    <row r="16" spans="2:3" s="58" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B16" s="61" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="62" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B18" s="59"/>
-    </row>
-    <row r="19" spans="2:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="B19" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Gantt chart with new timeline dates.
Extend time for writing final report draft and shorten time for
for doing preliminary powerpoint slides.
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\ENGR489\QuickCheck for Whiley\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F1D348-C8DB-4591-BEBA-050FF38CC0BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5114CCD-60F9-4AAD-B527-2ABB98EEDA8B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$A$1:$IS$25</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">ProjectSchedule!$4:$6</definedName>
     <definedName name="task_end" localSheetId="0">ProjectSchedule!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">ProjectSchedule!$D1</definedName>
@@ -112,9 +112,6 @@
     <t>Trimester 2</t>
   </si>
   <si>
-    <t>Produce Bibliography</t>
-  </si>
-  <si>
     <t>Produce project proposal</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>Prepare slides for final presentation</t>
+  </si>
+  <si>
+    <t>Produce bibliography</t>
   </si>
 </sst>
 </file>
@@ -1220,9 +1220,9 @@
   </sheetPr>
   <dimension ref="A1:IS28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF19" sqref="AF19"/>
+      <selection pane="topRight" activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4254,7 +4254,7 @@
     <row r="9" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
       <c r="B9" s="31" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33">
@@ -4520,7 +4520,7 @@
     <row r="10" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
       <c r="B10" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33">
@@ -4786,7 +4786,7 @@
     <row r="11" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
       <c r="B11" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="33">
@@ -5052,7 +5052,7 @@
     <row r="12" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="33">
@@ -5318,7 +5318,7 @@
     <row r="13" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
       <c r="B13" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="33">
@@ -5581,7 +5581,7 @@
     <row r="14" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33">
@@ -6107,7 +6107,7 @@
     <row r="16" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="41">
@@ -6117,12 +6117,12 @@
         <v>43283</v>
       </c>
       <c r="F16" s="56">
-        <v>43297</v>
+        <v>43290</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25">
         <f t="shared" si="144"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I16" s="48"/>
       <c r="J16" s="48"/>
@@ -6373,17 +6373,17 @@
     <row r="17" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="41">
         <v>0</v>
       </c>
-      <c r="E17" s="55">
-        <v>43297</v>
+      <c r="E17" s="56">
+        <v>43290</v>
       </c>
       <c r="F17" s="56">
-        <v>43318</v>
+        <v>43311</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25">
@@ -6639,14 +6639,14 @@
     <row r="18" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
       <c r="B18" s="39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="41">
         <v>0</v>
       </c>
       <c r="E18" s="56">
-        <v>43318</v>
+        <v>43311</v>
       </c>
       <c r="F18" s="56">
         <v>43358</v>
@@ -6654,7 +6654,7 @@
       <c r="G18" s="25"/>
       <c r="H18" s="25">
         <f t="shared" si="144"/>
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I18" s="48"/>
       <c r="J18" s="48"/>
@@ -6905,7 +6905,7 @@
     <row r="19" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="41">
@@ -7171,7 +7171,7 @@
     <row r="20" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
       <c r="B20" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="41">
@@ -7434,7 +7434,7 @@
     <row r="21" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
       <c r="B21" s="39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="41">
@@ -8748,6 +8748,33 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="IF4:IL4"/>
+    <mergeCell ref="IM4:IS4"/>
+    <mergeCell ref="GW4:HC4"/>
+    <mergeCell ref="HD4:HJ4"/>
+    <mergeCell ref="HK4:HQ4"/>
+    <mergeCell ref="HR4:HX4"/>
+    <mergeCell ref="HY4:IE4"/>
+    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="FU4:GA4"/>
+    <mergeCell ref="GB4:GH4"/>
+    <mergeCell ref="GI4:GO4"/>
+    <mergeCell ref="GP4:GV4"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="EZ4:FF4"/>
+    <mergeCell ref="FG4:FM4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
@@ -8757,33 +8784,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="EZ4:FF4"/>
-    <mergeCell ref="FG4:FM4"/>
-    <mergeCell ref="FN4:FT4"/>
-    <mergeCell ref="FU4:GA4"/>
-    <mergeCell ref="GB4:GH4"/>
-    <mergeCell ref="GI4:GO4"/>
-    <mergeCell ref="GP4:GV4"/>
-    <mergeCell ref="IF4:IL4"/>
-    <mergeCell ref="IM4:IS4"/>
-    <mergeCell ref="GW4:HC4"/>
-    <mergeCell ref="HD4:HJ4"/>
-    <mergeCell ref="HK4:HQ4"/>
-    <mergeCell ref="HR4:HX4"/>
-    <mergeCell ref="HY4:IE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D25">
     <cfRule type="dataBar" priority="54">
@@ -8830,8 +8830,8 @@
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="3" scale="26" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter scaleWithDoc="0"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>

</xml_diff>

<commit_message>
Fix typos in project proposal.
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\ENGR489\QuickCheck for Whiley\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5114CCD-60F9-4AAD-B527-2ABB98EEDA8B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E827A068-E58F-46DF-B692-CD73C491E90A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,16 +115,10 @@
     <t>Produce project proposal</t>
   </si>
   <si>
-    <t>Implement for types: bool, byte, int, real, null</t>
-  </si>
-  <si>
     <t>Produce preliminary report</t>
   </si>
   <si>
     <t>Extend automatic test generator</t>
-  </si>
-  <si>
-    <t>Implement for types: void, array, union and records</t>
   </si>
   <si>
     <t>Produce slides for presentation of preliminary report</t>
@@ -146,6 +140,12 @@
   </si>
   <si>
     <t>Produce bibliography</t>
+  </si>
+  <si>
+    <t>Implement for primitive types: bool, byte, int, null</t>
+  </si>
+  <si>
+    <t>Implement for complex types: void, array, union and records</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1222,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W22" sqref="W22"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4254,7 +4254,7 @@
     <row r="9" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
       <c r="B9" s="31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33">
@@ -4786,7 +4786,7 @@
     <row r="11" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
       <c r="B11" s="31" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="33">
@@ -5052,7 +5052,7 @@
     <row r="12" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="31" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="33">
@@ -5318,7 +5318,7 @@
     <row r="13" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
       <c r="B13" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="33">
@@ -5581,7 +5581,7 @@
     <row r="14" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33">
@@ -6107,7 +6107,7 @@
     <row r="16" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="41">
@@ -6373,7 +6373,7 @@
     <row r="17" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="39" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="41">
@@ -6639,7 +6639,7 @@
     <row r="18" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
       <c r="B18" s="39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="41">
@@ -6905,7 +6905,7 @@
     <row r="19" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="41">
@@ -7171,7 +7171,7 @@
     <row r="20" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
       <c r="B20" s="39" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="41">
@@ -7434,7 +7434,7 @@
     <row r="21" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
       <c r="B21" s="39" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="41">
@@ -8748,33 +8748,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="IF4:IL4"/>
-    <mergeCell ref="IM4:IS4"/>
-    <mergeCell ref="GW4:HC4"/>
-    <mergeCell ref="HD4:HJ4"/>
-    <mergeCell ref="HK4:HQ4"/>
-    <mergeCell ref="HR4:HX4"/>
-    <mergeCell ref="HY4:IE4"/>
-    <mergeCell ref="FN4:FT4"/>
-    <mergeCell ref="FU4:GA4"/>
-    <mergeCell ref="GB4:GH4"/>
-    <mergeCell ref="GI4:GO4"/>
-    <mergeCell ref="GP4:GV4"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="EZ4:FF4"/>
-    <mergeCell ref="FG4:FM4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
@@ -8784,6 +8757,33 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="EZ4:FF4"/>
+    <mergeCell ref="FG4:FM4"/>
+    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="FU4:GA4"/>
+    <mergeCell ref="GB4:GH4"/>
+    <mergeCell ref="GI4:GO4"/>
+    <mergeCell ref="GP4:GV4"/>
+    <mergeCell ref="IF4:IL4"/>
+    <mergeCell ref="IM4:IS4"/>
+    <mergeCell ref="GW4:HC4"/>
+    <mergeCell ref="HD4:HJ4"/>
+    <mergeCell ref="HK4:HQ4"/>
+    <mergeCell ref="HR4:HX4"/>
+    <mergeCell ref="HY4:IE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D25">
     <cfRule type="dataBar" priority="54">

</xml_diff>

<commit_message>
Modify Gantt chart based on future plan
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\ENGR489\QuickCheck for Whiley\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E827A068-E58F-46DF-B692-CD73C491E90A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7E569F-4A93-444E-8F73-B1072DFE4BA9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,19 +118,10 @@
     <t>Produce preliminary report</t>
   </si>
   <si>
-    <t>Extend automatic test generator</t>
-  </si>
-  <si>
     <t>Produce slides for presentation of preliminary report</t>
   </si>
   <si>
-    <t>Extend the automatic test generator</t>
-  </si>
-  <si>
     <t>Produce draft of final report</t>
-  </si>
-  <si>
-    <t>Complete implementation</t>
   </si>
   <si>
     <t>Finalise final report</t>
@@ -146,6 +137,15 @@
   </si>
   <si>
     <t>Implement for complex types: void, array, union and records</t>
+  </si>
+  <si>
+    <t>Evaluate tool</t>
+  </si>
+  <si>
+    <t>Add mutation testing on Whiley files</t>
+  </si>
+  <si>
+    <t>Optimise function/method calls</t>
   </si>
 </sst>
 </file>
@@ -1220,9 +1220,9 @@
   </sheetPr>
   <dimension ref="A1:IS28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4254,11 +4254,11 @@
     <row r="9" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
       <c r="B9" s="31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="53">
         <v>43178</v>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="53">
         <v>43178</v>
@@ -4786,11 +4786,11 @@
     <row r="11" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
       <c r="B11" s="31" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="53">
         <v>43178</v>
@@ -5052,11 +5052,11 @@
     <row r="12" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="54">
         <v>43206</v>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="33">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E13" s="53">
         <v>43234</v>
@@ -5581,7 +5581,7 @@
     <row r="14" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="31" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33">
@@ -6107,7 +6107,7 @@
     <row r="16" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="41">
@@ -6373,7 +6373,7 @@
     <row r="17" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="39" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="41">
@@ -6639,7 +6639,7 @@
     <row r="18" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
       <c r="B18" s="39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="41">
@@ -6905,7 +6905,7 @@
     <row r="19" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="39" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="41">
@@ -7171,7 +7171,7 @@
     <row r="20" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
       <c r="B20" s="39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="41">
@@ -7434,7 +7434,7 @@
     <row r="21" spans="1:253" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
       <c r="B21" s="39" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="41">
@@ -8748,6 +8748,33 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="IF4:IL4"/>
+    <mergeCell ref="IM4:IS4"/>
+    <mergeCell ref="GW4:HC4"/>
+    <mergeCell ref="HD4:HJ4"/>
+    <mergeCell ref="HK4:HQ4"/>
+    <mergeCell ref="HR4:HX4"/>
+    <mergeCell ref="HY4:IE4"/>
+    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="FU4:GA4"/>
+    <mergeCell ref="GB4:GH4"/>
+    <mergeCell ref="GI4:GO4"/>
+    <mergeCell ref="GP4:GV4"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="EZ4:FF4"/>
+    <mergeCell ref="FG4:FM4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
@@ -8757,33 +8784,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="EZ4:FF4"/>
-    <mergeCell ref="FG4:FM4"/>
-    <mergeCell ref="FN4:FT4"/>
-    <mergeCell ref="FU4:GA4"/>
-    <mergeCell ref="GB4:GH4"/>
-    <mergeCell ref="GI4:GO4"/>
-    <mergeCell ref="GP4:GV4"/>
-    <mergeCell ref="IF4:IL4"/>
-    <mergeCell ref="IM4:IS4"/>
-    <mergeCell ref="GW4:HC4"/>
-    <mergeCell ref="HD4:HJ4"/>
-    <mergeCell ref="HK4:HQ4"/>
-    <mergeCell ref="HR4:HX4"/>
-    <mergeCell ref="HY4:IE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D25">
     <cfRule type="dataBar" priority="54">

</xml_diff>